<commit_message>
Change Test.xlsx config file
</commit_message>
<xml_diff>
--- a/src/test/resources/kas/excel/Test.xlsx
+++ b/src/test/resources/kas/excel/Test.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900DF71C-F03E-4CC8-B663-9FAC5A6F3DAF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF63BC98-362F-4F0F-94E2-71A400F26E11}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DESCRIPTION" sheetId="2" r:id="rId1"/>
     <sheet name="PATTERN" sheetId="1" r:id="rId2"/>
-    <sheet name="ЩО-2.1-1" sheetId="4" r:id="rId3"/>
-    <sheet name="ЩО-2.1-2" sheetId="5" r:id="rId4"/>
+    <sheet name="Нормальный" sheetId="4" r:id="rId3"/>
+    <sheet name="Криворукий" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="диммирование">DESCRIPTION!$C$16:$C$17</definedName>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
-  <si>
-    <t>IP Контроллера Helvar:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Номер помещения</t>
   </si>
@@ -61,18 +58,9 @@
     <t>34D</t>
   </si>
   <si>
-    <t>да</t>
-  </si>
-  <si>
     <t>10.119.140.87</t>
   </si>
   <si>
-    <t>Щит контроллера Helvar:</t>
-  </si>
-  <si>
-    <t>Номер котроллера Helvar:</t>
-  </si>
-  <si>
     <t>Принципы успешной работы с файлом:</t>
   </si>
   <si>
@@ -149,6 +137,18 @@
   </si>
   <si>
     <t>Helvar group number</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>Значение для группы освещения без диммирования:</t>
+  </si>
+  <si>
+    <t>Значение для группы освещения с диммированием:</t>
   </si>
 </sst>
 </file>
@@ -193,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,9 +206,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -499,7 +496,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +507,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -518,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -526,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -534,7 +531,7 @@
         <v>2.1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -542,7 +539,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -550,7 +547,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -566,7 +563,7 @@
         <v>3.1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,7 +571,7 @@
         <v>3.2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -582,7 +579,7 @@
         <v>3.3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,7 +587,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,7 +595,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -606,7 +603,7 @@
         <v>4.2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,7 +611,7 @@
         <v>4.3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -622,17 +619,29 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="C16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -643,11 +652,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,91 +668,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
+      <c r="A2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>257</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>286</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>287</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Допустимые значения:" prompt="&quot;нет&quot; - если группа освещения без диммирования_x000a_&quot;да&quot; - если группа освещения с диммированием" sqref="D6:D1048576" xr:uid="{FE596FE9-D262-4DB8-A4B5-D80FA1EED29E}">
-      <formula1>"диммирование"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Допустимые значения:" prompt="&quot;нет&quot; - если группа освещения без диммирования_x000a_&quot;да&quot; - если группа освещения с диммированием" sqref="D5" xr:uid="{2C4BE783-E026-4A4E-8A29-BBFC8BCD13D4}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D1048576" xr:uid="{223F74B7-0392-4C46-9D64-7C685346A9DB}">
       <formula1>диммирование</formula1>
     </dataValidation>
   </dataValidations>
@@ -771,32 +769,32 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>37</v>
+      <c r="B3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,13 +802,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,13 +816,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -832,13 +830,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -854,91 +852,93 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11218953-FA0D-49FE-911B-9B3F6BC1BC92}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>257</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>286</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>287</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>287</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>